<commit_message>
feat: save generated property values and used group hashes
</commit_message>
<xml_diff>
--- a/generated_property_values.xlsx
+++ b/generated_property_values.xlsx
@@ -7,7 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="是否精华" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="结束时间" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="开始时间" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="收货日期" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="联系电话" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="开票时间" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="会议时间" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="备注" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="是否精华" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="公告时间" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,77 +444,768 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>是否精华</t>
+          <t>结束时间</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>2020年12月31日</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>2021年5月20日</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>2022年1月1日</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>2023年9月30日</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>2024年6月15日</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>2025年3月10日</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>2026年11月25日</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>2027年8月5日</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>2028年2月29日</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>2030年7月10日</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>开始时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2020年1月1日</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2019年5月15日</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022年3月10日</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018年9月30日</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023年7月20日</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2017年12月25日</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024年8月5日</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2016年4月12日</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025年11月18日</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2015年10月3日</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>收货日期</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1月1日</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3月15日</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5月10日</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>7月22日</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>9月5日</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11月11日</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2月28日</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>4月20日</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6月8日</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>12月31日</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>联系电话</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>9876543210</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1357924680</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2468135790</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3698521470</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2587413690</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1472583690</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>6547893210</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9874561230</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>7418529630</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>开票时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2020年1月1日</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2019年10月15日</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021年3月20日</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018年5月6日</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022年12月31日</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2017年8月25日</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2016年4月10日</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2015年11月11日</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2014年7月2日</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2013年9月18日</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>会议时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>9:00 am</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>10:30 am</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2:00 pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3:45 pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5:15 pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6:30 pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>8:00 am</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>11:45 am</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>4:30 pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>7:15 pm</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>备注</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>抱歉，这是10个姓名的示例值。如果您需要其他属性的示例，请提供相关信息。</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>是否精华</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>否，是</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>公告时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2020-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2020-03-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2020-04-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2020-05-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2020-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2020-07-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2020-08-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2020-09</t>
         </is>
       </c>
     </row>

</xml_diff>